<commit_message>
Fixing issue with matching
</commit_message>
<xml_diff>
--- a/excel_input.xlsx
+++ b/excel_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f45f2a6c0e1abdcf/Dokumente/Count_prototype/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\OneDrive\Dokumente\Count_prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{A95D2FA6-BE41-4B93-B538-DDFC5A2A516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32CA6F5E-A1FA-4257-94A4-00C97D1AE6CB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED99547F-DF8A-42CD-AD82-94E0FAE945AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20025" yWindow="1110" windowWidth="28080" windowHeight="15300" xr2:uid="{644204C7-A476-464E-8C4D-A7FD18C7D8D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{644204C7-A476-464E-8C4D-A7FD18C7D8D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>quantity</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Grano Padano</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>Kasseler</t>
   </si>
   <si>
@@ -58,6 +55,141 @@
   </si>
   <si>
     <t>Haferdrink</t>
+  </si>
+  <si>
+    <t>Botato Ofenkroketten</t>
+  </si>
+  <si>
+    <t>Tomaten 500g VKE</t>
+  </si>
+  <si>
+    <t>Gurken ST</t>
+  </si>
+  <si>
+    <t>LMUV H-Sahne</t>
+  </si>
+  <si>
+    <t>Parmigiano</t>
+  </si>
+  <si>
+    <t>Italia Pasta</t>
+  </si>
+  <si>
+    <t>Markenbutter</t>
+  </si>
+  <si>
+    <t>LMUV Naturjog.</t>
+  </si>
+  <si>
+    <t>Bandnud.</t>
+  </si>
+  <si>
+    <t>Miniplaumentom.</t>
+  </si>
+  <si>
+    <t>Orangen lose aus der Box</t>
+  </si>
+  <si>
+    <t>Bio Zitronen</t>
+  </si>
+  <si>
+    <t>Tomate Cherryrom</t>
+  </si>
+  <si>
+    <t>Pliz Champign</t>
+  </si>
+  <si>
+    <t>Pe sto Ricotta</t>
+  </si>
+  <si>
+    <t>Spaetzle</t>
+  </si>
+  <si>
+    <t>Porree</t>
+  </si>
+  <si>
+    <t>Emm entaler Ger.</t>
+  </si>
+  <si>
+    <t>Rohschinken Gew.</t>
+  </si>
+  <si>
+    <t>Creme Fraiche</t>
+  </si>
+  <si>
+    <t>Oberkeulensteaks</t>
+  </si>
+  <si>
+    <t>Kart. Drillinge</t>
+  </si>
+  <si>
+    <t>Eisbergsalat</t>
+  </si>
+  <si>
+    <t>Tr. Hell Kernl.</t>
+  </si>
+  <si>
+    <t>Gouda alt SHB</t>
+  </si>
+  <si>
+    <t>Gusto Pizza pros.</t>
+  </si>
+  <si>
+    <t>Pecorino romano</t>
+  </si>
+  <si>
+    <t>Eier Nrw</t>
+  </si>
+  <si>
+    <t>Tomaten Treimix</t>
+  </si>
+  <si>
+    <t>VV la. H-Milch</t>
+  </si>
+  <si>
+    <t>Spagettini</t>
+  </si>
+  <si>
+    <t>Mandarinen 1Kg VKE</t>
+  </si>
+  <si>
+    <t>M.I. Mozarella</t>
+  </si>
+  <si>
+    <t>Havana Club 3 Jahre</t>
+  </si>
+  <si>
+    <t>Kornw. Weizenm.</t>
+  </si>
+  <si>
+    <t>Bio BB Zitr.</t>
+  </si>
+  <si>
+    <t>Bio Rispentom.</t>
+  </si>
+  <si>
+    <t>H-Brustfilet</t>
+  </si>
+  <si>
+    <t>Fri. Mil</t>
+  </si>
+  <si>
+    <t>Möhren Bio</t>
+  </si>
+  <si>
+    <t>Käsetheke Pfeffer</t>
+  </si>
+  <si>
+    <t>Bio Sojadrink Natur</t>
+  </si>
+  <si>
+    <t>Bio Feta 45%</t>
+  </si>
+  <si>
+    <t>Weidebutter Suess</t>
+  </si>
+  <si>
+    <t>product</t>
   </si>
 </sst>
 </file>
@@ -409,17 +541,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE889B18-8494-4D11-8D17-A8F623F46AE5}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A39" sqref="A34:A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -451,7 +586,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -459,7 +594,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -467,9 +602,361 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
         <v>1</v>
       </c>
     </row>

</xml_diff>